<commit_message>
update in attendance feature
</commit_message>
<xml_diff>
--- a/ICT.xlsx
+++ b/ICT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\attandance_pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Course</t>
   </si>
@@ -62,13 +62,58 @@
     <t>PRESENT</t>
   </si>
   <si>
+    <t>Finanace</t>
+  </si>
+  <si>
+    <t>arts&amp;crafts</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>G-11</t>
+  </si>
+  <si>
+    <t>marwa</t>
+  </si>
+  <si>
+    <t>jabeen</t>
+  </si>
+  <si>
+    <t>husnain</t>
+  </si>
+  <si>
+    <t>ahmad</t>
+  </si>
+  <si>
+    <t>URDU</t>
+  </si>
+  <si>
+    <t>urdu</t>
+  </si>
+  <si>
+    <t>alisha</t>
+  </si>
+  <si>
+    <t>Fatima</t>
+  </si>
+  <si>
+    <t>ICT</t>
+  </si>
+  <si>
+    <t>Atiqa</t>
+  </si>
+  <si>
     <t>Tabbasum</t>
   </si>
   <si>
     <t>shaista</t>
   </si>
   <si>
-    <t>ICT</t>
+    <t>Cs</t>
+  </si>
+  <si>
+    <t>tabbasum</t>
   </si>
   <si>
     <t>Teacher First Name</t>
@@ -80,34 +125,25 @@
     <t>atiqa</t>
   </si>
   <si>
-    <t>cs</t>
-  </si>
-  <si>
-    <t>F-18</t>
-  </si>
-  <si>
-    <t>english</t>
+    <t>anfal</t>
   </si>
   <si>
     <t>math</t>
   </si>
   <si>
-    <t>F-11</t>
-  </si>
-  <si>
-    <t>absent</t>
-  </si>
-  <si>
-    <t>Anfal</t>
-  </si>
-  <si>
-    <t>fatima</t>
-  </si>
-  <si>
-    <t>junaid</t>
-  </si>
-  <si>
-    <t>anwer</t>
+    <t xml:space="preserve">maham </t>
+  </si>
+  <si>
+    <t>masoom</t>
+  </si>
+  <si>
+    <t>ibtasam</t>
+  </si>
+  <si>
+    <t>ilahi</t>
+  </si>
+  <si>
+    <t>Lalain</t>
   </si>
 </sst>
 </file>
@@ -457,7 +493,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +502,7 @@
     <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,18 +528,18 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2">
         <v>45541</v>
@@ -512,111 +548,183 @@
         <v>45505</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="C3" s="2">
+        <v>45528</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45527</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45541</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45505</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="2">
-        <v>45542</v>
+        <v>45530</v>
       </c>
       <c r="D4" s="2">
         <v>45505</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45528</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45505</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45541</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45505</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
+    <row r="7" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45528</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45505</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>